<commit_message>
updated to changes: Path = Parent + Name. Previously, Path was considered as parent.
</commit_message>
<xml_diff>
--- a/EquipmentModelBulkLoadTool/ProtocolsExamples.xlsx
+++ b/EquipmentModelBulkLoadTool/ProtocolsExamples.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ABB_Work\Examples\EquipmentModelBulkLoadTool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Examples\EquipmentModelBulkLoadTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE183058-1264-47D6-B91A-2DFF11D01513}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8A6215-ED5D-498B-9E09-EA494BDE40B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{3E895CE0-B3EA-4AE3-B408-2B90AE8526E7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3E895CE0-B3EA-4AE3-B408-2B90AE8526E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Class: Tank</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Instance : Tank</t>
   </si>
   <si>
-    <t>Path</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>ahost</t>
   </si>
   <si>
-    <t>Clsid</t>
-  </si>
-  <si>
     <t>Source OPCDA3</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
     <t>opc.t.1</t>
   </si>
   <si>
-    <t>{91210ec1-58ac-41f9-b840-b39b965076fc}</t>
-  </si>
-  <si>
     <t>Test.Item.C1</t>
   </si>
   <si>
@@ -188,6 +179,15 @@
   </si>
   <si>
     <t>Access paths output:</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>ClsId</t>
+  </si>
+  <si>
+    <t>91210ec1-58ac-41f9-b840-b39b965076fc</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="C2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91210B48-3707-4D6E-850B-0BA81C67EAED}">
   <dimension ref="B3:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,80 +681,81 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
+      <c r="E3" s="2" t="str">
+        <f>Models!C3</f>
+        <v>Level</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="O3" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>11111</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>20</v>
@@ -763,143 +764,143 @@
         <v>22222</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" t="s">
         <v>44</v>
-      </c>
-      <c r="O6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7">
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8">
         <v>30</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F9">
         <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I9">
         <v>10001</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
       <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
         <v>36</v>
       </c>
-      <c r="H10" t="s">
-        <v>39</v>
-      </c>
       <c r="N10" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>